<commit_message>
Add combined developer report processing and budget calculations
</commit_message>
<xml_diff>
--- a/backend/mana_algo/proposals/dev_reports/HACKATHON_SHAWN_MANA_HOURS.xlsx
+++ b/backend/mana_algo/proposals/dev_reports/HACKATHON_SHAWN_MANA_HOURS.xlsx
@@ -1,57 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\BN3PEPF00008C1C\EXCELCNV\73079cee-921b-4eed-90d5-9075f81cf7b0\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{81CFDCD5-E543-45A5-AC1E-CBF9638BCDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54826D25-E041-4C51-848B-BC12533673BA}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="FYRE" sheetId="1" r:id="rId1"/>
-    <sheet name="SHLD" sheetId="2" r:id="rId2"/>
-    <sheet name="MANA" sheetId="3" r:id="rId3"/>
-    <sheet name="mana effort hours" sheetId="4" r:id="rId4"/>
-    <sheet name="mana hours to mana" sheetId="5" r:id="rId5"/>
-    <sheet name="MANA Governance" sheetId="6" r:id="rId6"/>
-    <sheet name="VicTory Exchange" sheetId="7" r:id="rId7"/>
-    <sheet name="Project Management" sheetId="8" r:id="rId8"/>
-    <sheet name="Server-PM" sheetId="9" r:id="rId9"/>
-    <sheet name="Content " sheetId="10" r:id="rId10"/>
+    <sheet name="FYRE" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SHLD" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="MANA" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="mana effort hours" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="mana hours to mana" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="MANA Governance" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="VicTory Exchange" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Project Management" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Server-PM" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Content " sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Content '!$A$1:$H$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FYRE!$B$1:$H$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MANA!$A$1:$H$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'mana effort hours'!$A$1:$H$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'MANA Governance'!$A$1:$H$26</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'mana hours to mana'!$A$1:$H$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Project Management'!$A$1:$H$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Server-PM'!$A$1:$H$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SHLD!$A$1:$H$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'VicTory Exchange'!$A$1:$H$20</definedName>
+    <definedName function="false" hidden="true" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'Content '!$A$1:$H$6</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">FYRE!$B$1:$H$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">MANA!$A$1:$H$12</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'mana effort hours'!$A$1:$H$15</definedName>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'MANA Governance'!$A$1:$H$26</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'mana hours to mana'!$A$1:$H$21</definedName>
+    <definedName function="false" hidden="true" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">'Project Management'!$A$1:$H$5</definedName>
+    <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">'Server-PM'!$A$1:$H$4</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">SHLD!$A$1:$H$10</definedName>
+    <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">'VicTory Exchange'!$A$1:$H$20</definedName>
   </definedNames>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -62,566 +43,569 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="185">
   <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>Subproject</t>
-  </si>
-  <si>
-    <t>Epic</t>
-  </si>
-  <si>
-    <t>Story</t>
-  </si>
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>Estimated Hours</t>
-  </si>
-  <si>
-    <t>Budgeted</t>
-  </si>
-  <si>
-    <t>Actual Hours</t>
-  </si>
-  <si>
-    <t>Blockchain Developer</t>
-  </si>
-  <si>
-    <t>Token Contracts</t>
-  </si>
-  <si>
-    <t>FYRE</t>
-  </si>
-  <si>
-    <t>User Story #1: ERC-20 Token Implementation</t>
-  </si>
-  <si>
-    <t>- Implement ERC-20 Token Contract for FYRE</t>
-  </si>
-  <si>
-    <t>- Add Minting, Burning, and Transferring Functions</t>
-  </si>
-  <si>
-    <t>- Test Standard Token Operations</t>
-  </si>
-  <si>
-    <t>User Story #4: SHLD Interaction with FYRE</t>
-  </si>
-  <si>
-    <t>- Develop FYRE Conversion Functions for SHLD Purchase</t>
-  </si>
-  <si>
-    <t>- Implement FYRE to MANA Conversion Mechanism</t>
-  </si>
-  <si>
-    <t>- Define and Code Governance Rules for FYRE Usage</t>
-  </si>
-  <si>
-    <t>- User Interface Development for Conversion Processes</t>
-  </si>
-  <si>
-    <t>- Testing and Security Review</t>
-  </si>
-  <si>
-    <t>SHLD</t>
-  </si>
-  <si>
-    <t>User Story #1: NEAR NFT Implementation for SHLD</t>
-  </si>
-  <si>
-    <t>- Develop ERC-721 Contract for Non-Transferable SHLD</t>
-  </si>
-  <si>
-    <t>- On-Chain Metadata Storage</t>
-  </si>
-  <si>
-    <t>- Testing Non-Transferable NFT Features</t>
-  </si>
-  <si>
-    <t>User Story #2: Governance Voting for SHLD Holders</t>
-  </si>
-  <si>
-    <t>- Develop Governance Voting Smart Contracts</t>
-  </si>
-  <si>
-    <t>- Integrate SHLD Voting into Governance</t>
-  </si>
-  <si>
-    <t>- Testing Governance Voting Mechanism</t>
-  </si>
-  <si>
-    <t>User Story #3: Project Contribution Voting</t>
-  </si>
-  <si>
-    <t>- Develop Project Contribution Voting Contracts</t>
-  </si>
-  <si>
-    <t>- Integrate Voting with Project Budgets</t>
-  </si>
-  <si>
-    <t>- Testing Project Voting and Budget Approval</t>
-  </si>
-  <si>
-    <t>MANA</t>
-  </si>
-  <si>
-    <t>User Story #1: MANA Token Lifecycle Starting as ERC-20 Token</t>
-  </si>
-  <si>
-    <t>- Implement ERC-20 Token Contract for MANA</t>
-  </si>
-  <si>
-    <t>- Develop Contribution Mechanism</t>
-  </si>
-  <si>
-    <t>- Transition from ERC-20 to ERC-1400 upon Contribution</t>
-  </si>
-  <si>
-    <t>- Test ERC-20 to ERC-1400 Transition Workflow</t>
-  </si>
-  <si>
-    <t>User Story #2: ERC-1400 MANA Token Implementation</t>
-  </si>
-  <si>
-    <t>- Develop ERC-1400 Contract for MANA</t>
-  </si>
-  <si>
-    <t>- Implement Divisibility and Partition Features</t>
-  </si>
-  <si>
-    <t>- Test ERC-1400 Token Functionality</t>
-  </si>
-  <si>
-    <t>User Story #3: Governance and Project Voting</t>
-  </si>
-  <si>
-    <t>- Develop Voting Smart Contracts for MANA</t>
-  </si>
-  <si>
-    <t>- Integrate MANA Voting into Cooperative Governance</t>
-  </si>
-  <si>
-    <t>- Project Allocation Voting with MANA</t>
-  </si>
-  <si>
-    <t>- Test Governance and Project Voting</t>
-  </si>
-  <si>
-    <t>Frontend Developer</t>
-  </si>
-  <si>
-    <t>Mana DApp</t>
-  </si>
-  <si>
-    <t>mana hour tracking</t>
-  </si>
-  <si>
-    <t>Log Hours Worked</t>
-  </si>
-  <si>
-    <t>Implement basic input fields</t>
-  </si>
-  <si>
-    <t>Backend Developer</t>
-  </si>
-  <si>
-    <t>Store logged hours in a secure database</t>
-  </si>
-  <si>
-    <t>Ensure logged hours exported</t>
-  </si>
-  <si>
-    <t>Log Hours Worked Proofs</t>
-  </si>
-  <si>
-    <t>Record proof of work (hours logged) on-chain</t>
-  </si>
-  <si>
-    <t>Display Allocated MANA Hours</t>
-  </si>
-  <si>
-    <t>Implement dashboard</t>
-  </si>
-  <si>
-    <t>Fetch data from the project manager's MANA sheet</t>
-  </si>
-  <si>
-    <t>Log final MANA allocation on-chain</t>
-  </si>
-  <si>
-    <t>Generate Report for Project Manager</t>
-  </si>
-  <si>
-    <t>Develop report generation feature</t>
-  </si>
-  <si>
-    <t>Display discrepancies</t>
-  </si>
-  <si>
-    <t>Export report as spreadsheet/PDF</t>
-  </si>
-  <si>
-    <t>Store final report on-chain</t>
-  </si>
-  <si>
-    <t>Basic Display for Effort Tracking</t>
-  </si>
-  <si>
-    <t>Create front-end display</t>
-  </si>
-  <si>
-    <t>Compare tracked hours with allocated MANA</t>
-  </si>
-  <si>
-    <t>Record final tracked hours on-chain</t>
-  </si>
-  <si>
-    <t>mana algorithm</t>
-  </si>
-  <si>
-    <t>Setup Project MANA Allocation</t>
-  </si>
-  <si>
-    <t>Define total MANA allocation</t>
-  </si>
-  <si>
-    <t>Record final allocation on-chain</t>
-  </si>
-  <si>
-    <t>Calculate Role-Based Multipliers</t>
-  </si>
-  <si>
-    <t>Calculate the weighted average pay rate</t>
-  </si>
-  <si>
-    <t>Log final multiplier values on-chain</t>
-  </si>
-  <si>
-    <t>Set up hour tracking</t>
-  </si>
-  <si>
-    <t>Record logged hours on-chain</t>
-  </si>
-  <si>
-    <t>Calculate MANA Per Hour</t>
-  </si>
-  <si>
-    <t>Calculate MANA per hour</t>
-  </si>
-  <si>
-    <t>Log MANA per hour on-chain</t>
-  </si>
-  <si>
-    <t>Conduct 360-Degree Peer Voting</t>
-  </si>
-  <si>
-    <t>Set up peer voting system</t>
-  </si>
-  <si>
-    <t>Store peer voting results on-chain</t>
-  </si>
-  <si>
-    <t>Implement Confidence Interval</t>
-  </si>
-  <si>
-    <t>Set up confidence intervals</t>
-  </si>
-  <si>
-    <t>Record confidence intervals on-chain</t>
-  </si>
-  <si>
-    <t>Apply Pay Rate Modifier</t>
-  </si>
-  <si>
-    <t>Apply pay rate modifier</t>
-  </si>
-  <si>
-    <t>Log pay rate modifications on-chain</t>
-  </si>
-  <si>
-    <t>Apply Stakeholder Multiplier</t>
-  </si>
-  <si>
-    <t>Create stakeholder evaluation rubric</t>
-  </si>
-  <si>
-    <t>Log stakeholder evaluations on-chain</t>
-  </si>
-  <si>
-    <t>Implement Feedback System</t>
-  </si>
-  <si>
-    <t>Develop feedback system</t>
-  </si>
-  <si>
-    <t>Store feedback on-chain</t>
-  </si>
-  <si>
-    <t>Apply Final Scaling</t>
-  </si>
-  <si>
-    <t>Apply final scaling</t>
-  </si>
-  <si>
-    <t>Log final scaling on-chain</t>
-  </si>
-  <si>
-    <t>MANA Governance</t>
-  </si>
-  <si>
-    <t>Voting Mechanism</t>
-  </si>
-  <si>
-    <t>Implement voting UI</t>
-  </si>
-  <si>
-    <t>Develop backend logic</t>
-  </si>
-  <si>
-    <t>Implement voting on-chain</t>
-  </si>
-  <si>
-    <t>Project Manager</t>
-  </si>
-  <si>
-    <t>Test voting mechanism</t>
-  </si>
-  <si>
-    <t>Proposal Submission</t>
-  </si>
-  <si>
-    <t>Create proposal submission form</t>
-  </si>
-  <si>
-    <t>Store/retrieve proposals</t>
-  </si>
-  <si>
-    <t>Record proposals on-chain</t>
-  </si>
-  <si>
-    <t>Review submissions</t>
-  </si>
-  <si>
-    <t>Governance Voting Report Generation</t>
-  </si>
-  <si>
-    <t>Develop report generation</t>
-  </si>
-  <si>
-    <t>Export report</t>
-  </si>
-  <si>
-    <t>Store report on-chain</t>
-  </si>
-  <si>
-    <t>Finalize report</t>
-  </si>
-  <si>
-    <t>Displaying MANA Allocations</t>
-  </si>
-  <si>
-    <t>Create display for MANA allocations</t>
-  </si>
-  <si>
-    <t>Fetch MANA allocation data</t>
-  </si>
-  <si>
-    <t>Record MANA allocations on-chain</t>
-  </si>
-  <si>
-    <t>Ensure accuracy of MANA allocations</t>
-  </si>
-  <si>
-    <t>Project Governance Voting</t>
-  </si>
-  <si>
-    <t>Implement project governance UI</t>
-  </si>
-  <si>
-    <t>Backend logic for project voting</t>
-  </si>
-  <si>
-    <t>Record project voting on-chain</t>
-  </si>
-  <si>
-    <t>MANA Hours-to-MANA Conversion</t>
-  </si>
-  <si>
-    <t>Implement conversion UI</t>
-  </si>
-  <si>
-    <t>Backend logic for conversion</t>
-  </si>
-  <si>
-    <t>Record conversion on-chain</t>
-  </si>
-  <si>
-    <t>View Final MANA Results</t>
-  </si>
-  <si>
-    <t>Create results dashboard</t>
-  </si>
-  <si>
-    <t>Fetch MANA results</t>
-  </si>
-  <si>
-    <t>Log final project hours on-chain</t>
-  </si>
-  <si>
-    <t>VicTory Exchange</t>
-  </si>
-  <si>
-    <t>FYRE Purchase Interface</t>
-  </si>
-  <si>
-    <t>Connect Wallet</t>
-  </si>
-  <si>
-    <t>Create FYRE Purchase Interface</t>
-  </si>
-  <si>
-    <t>Display Token Prices and Supply Stats</t>
-  </si>
-  <si>
-    <t>SHLD Purchase Simulation</t>
-  </si>
-  <si>
-    <t>Check FYRE Balance</t>
-  </si>
-  <si>
-    <t>Create SHLD Purchase Interface</t>
-  </si>
-  <si>
-    <t>AI-Generated Customization for SHLD NFTs</t>
-  </si>
-  <si>
-    <t>MANA Contribution Interface</t>
-  </si>
-  <si>
-    <t>Create MANA Contribution Interface</t>
-  </si>
-  <si>
-    <t>Setup MANA Contribution API</t>
-  </si>
-  <si>
-    <t>MANA to FYRE Conversion</t>
-  </si>
-  <si>
-    <t>Create MANA-to-FYRE Conversion Interface</t>
-  </si>
-  <si>
-    <t>Setup Conversion Logic and API</t>
-  </si>
-  <si>
-    <t>MANA Collateralization</t>
-  </si>
-  <si>
-    <t>Create Collateralization Interface for MANA</t>
-  </si>
-  <si>
-    <t>Manage Collateralization Logic and API</t>
-  </si>
-  <si>
-    <t>Frontend and Backend Integration</t>
-  </si>
-  <si>
-    <t>Integrate Frontend Wallet and Purchase Logic</t>
-  </si>
-  <si>
-    <t>Test and Finalize Backend APIs</t>
-  </si>
-  <si>
-    <t>Overall Integration Testing</t>
-  </si>
-  <si>
-    <t>Project Management</t>
-  </si>
-  <si>
-    <t>Generate Token Contract Plans</t>
-  </si>
-  <si>
-    <t>Create plans for FYRE, SHLD, MANA</t>
-  </si>
-  <si>
-    <t>Generate MANA Dapp Plans</t>
-  </si>
-  <si>
-    <t>Create plan for mana effort tracking and governance system</t>
-  </si>
-  <si>
-    <t>Generate mana hr to mana algo</t>
-  </si>
-  <si>
-    <t>Create Algorithm for mana hours to mana conversions</t>
-  </si>
-  <si>
-    <t>Generate plan for mana hr to mana algo</t>
-  </si>
-  <si>
-    <t>Create plan for mana hours to mana conversion</t>
-  </si>
-  <si>
-    <t>Server</t>
-  </si>
-  <si>
-    <t>Backend Template</t>
-  </si>
-  <si>
-    <t>Create backend template for MANA Dapp</t>
-  </si>
-  <si>
-    <t>Create backend template for Vicotry Dapp</t>
-  </si>
-  <si>
-    <t>Depoy Taiga</t>
-  </si>
-  <si>
-    <t>Deploy Taiga on Server</t>
-  </si>
-  <si>
-    <t>Content Developer</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
-    <t>Website Landing Page</t>
-  </si>
-  <si>
-    <t>Create website template</t>
-  </si>
-  <si>
-    <t>Victory Dapp Pages (FYRE SHLD, MANA)</t>
-  </si>
-  <si>
-    <t>Create Victory Dapp Templates</t>
-  </si>
-  <si>
-    <t>MANA Dapp Landing Page</t>
-  </si>
-  <si>
-    <t>Create Mana DApp Templates</t>
-  </si>
-  <si>
-    <t>Website Content</t>
+    <t xml:space="preserve">Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subproject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Budgeted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blockchain Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Token Contracts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FYRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Story #1: ERC-20 Token Implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Implement ERC-20 Token Contract for FYRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Add Minting, Burning, and Transferring Functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Test Standard Token Operations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Story #4: SHLD Interaction with FYRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Develop FYRE Conversion Functions for SHLD Purchase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Implement FYRE to MANA Conversion Mechanism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Define and Code Governance Rules for FYRE Usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- User Interface Development for Conversion Processes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Testing and Security Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Story #1: NEAR NFT Implementation for SHLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Develop ERC-721 Contract for Non-Transferable SHLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- On-Chain Metadata Storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Testing Non-Transferable NFT Features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Story #2: Governance Voting for SHLD Holders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Develop Governance Voting Smart Contracts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Integrate SHLD Voting into Governance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Testing Governance Voting Mechanism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Story #3: Project Contribution Voting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Develop Project Contribution Voting Contracts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Integrate Voting with Project Budgets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Testing Project Voting and Budget Approval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Story #1: MANA Token Lifecycle Starting as ERC-20 Token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Implement ERC-20 Token Contract for MANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Develop Contribution Mechanism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Transition from ERC-20 to ERC-1400 upon Contribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Test ERC-20 to ERC-1400 Transition Workflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Story #2: ERC-1400 MANA Token Implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Develop ERC-1400 Contract for MANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Implement Divisibility and Partition Features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Test ERC-1400 Token Functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Story #3: Governance and Project Voting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Develop Voting Smart Contracts for MANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Integrate MANA Voting into Cooperative Governance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Project Allocation Voting with MANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Test Governance and Project Voting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frontend Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mana DApp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mana hour tracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log Hours Worked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement basic input fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store logged hours in a secure database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensure logged hours exported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log Hours Worked Proofs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record proof of work (hours logged) on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display Allocated MANA Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fetch data from the project manager's MANA sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log final MANA allocation on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate Report for Project Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop report generation feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display discrepancies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Export report as spreadsheet/PDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store final report on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic Display for Effort Tracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create front-end display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compare tracked hours with allocated MANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record final tracked hours on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mana algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup Project MANA Allocation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Define total MANA allocation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record final allocation on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate Role-Based Multipliers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate the weighted average pay rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log final multiplier values on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set up hour tracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record logged hours on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate MANA Per Hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate MANA per hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log MANA per hour on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conduct 360-Degree Peer Voting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set up peer voting system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store peer voting results on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement Confidence Interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set up confidence intervals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record confidence intervals on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply Pay Rate Modifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply pay rate modifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log pay rate modifications on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply Stakeholder Multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create stakeholder evaluation rubric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log stakeholder evaluations on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement Feedback System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop feedback system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store feedback on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply Final Scaling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply final scaling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log final scaling on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANA Governance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voting Mechanism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement voting UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop backend logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement voting on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test voting mechanism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proposal Submission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create proposal submission form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store/retrieve proposals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record proposals on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review submissions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Governance Voting Report Generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop report generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Export report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store report on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalize report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Displaying MANA Allocations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create display for MANA allocations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fetch MANA allocation data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record MANA allocations on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensure accuracy of MANA allocations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Governance Voting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement project governance UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend logic for project voting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record project voting on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANA Hours-to-MANA Conversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement conversion UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend logic for conversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record conversion on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View Final MANA Results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create results dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fetch MANA results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log final project hours on-chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VicTory Exchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FYRE Purchase Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connect Wallet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create FYRE Purchase Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display Token Prices and Supply Stats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHLD Purchase Simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check FYRE Balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create SHLD Purchase Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-Generated Customization for SHLD NFTs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANA Contribution Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create MANA Contribution Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup MANA Contribution API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANA to FYRE Conversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create MANA-to-FYRE Conversion Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup Conversion Logic and API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANA Collateralization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Collateralization Interface for MANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manage Collateralization Logic and API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frontend and Backend Integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrate Frontend Wallet and Purchase Logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test and Finalize Backend APIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overall Integration Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate Token Contract Plans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create plans for FYRE, SHLD, MANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate MANA Dapp Plans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create plan for mana effort tracking and governance system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate mana hr to mana algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Algorithm for mana hours to mana conversions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate plan for mana hr to mana algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create plan for mana hours to mana conversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend Template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create backend template for MANA Dapp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create backend template for Vicotry Dapp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depoy Taiga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deploy Taiga on Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website Landing Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create website template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victory Dapp Pages (FYRE SHLD, MANA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Victory Dapp Templates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANA Dapp Landing Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Mana DApp Templates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website Content</t>
   </si>
   <si>
     <t xml:space="preserve">Create website content </t>
   </si>
   <si>
-    <t>UI/UX</t>
-  </si>
-  <si>
-    <t>Add UI/UX elements</t>
+    <t xml:space="preserve">UI/UX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add UI/UX elements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -630,22 +614,40 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -658,7 +660,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -666,358 +668,156 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF3D3D3D"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" customWidth="1"/>
-    <col min="5" max="5" width="49.42578125" customWidth="1"/>
-    <col min="6" max="7" width="17" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="49.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1043,7 +843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1059,12 +859,12 @@
       <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="5" t="n">
         <v>8</v>
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1080,12 +880,12 @@
       <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1101,12 +901,12 @@
       <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1122,12 +922,12 @@
       <c r="E5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="5" t="n">
         <v>12</v>
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1143,12 +943,12 @@
       <c r="E6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="5" t="n">
         <v>10</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1164,12 +964,12 @@
       <c r="E7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="5" t="n">
         <v>8</v>
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1185,12 +985,12 @@
       <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="5" t="n">
         <v>12</v>
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1206,38 +1006,47 @@
       <c r="E9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="5" t="n">
         <v>8</v>
       </c>
       <c r="G9" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:H9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:H9"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" customWidth="1"/>
-    <col min="6" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="49.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1263,7 +1072,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>173</v>
       </c>
@@ -1279,14 +1088,14 @@
       <c r="E2" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="4" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>173</v>
       </c>
@@ -1302,14 +1111,14 @@
       <c r="E3" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="4" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>173</v>
       </c>
@@ -1325,14 +1134,14 @@
       <c r="E4" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="4" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>173</v>
       </c>
@@ -1348,12 +1157,12 @@
       <c r="E5" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="4" t="n">
         <v>40</v>
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>173</v>
       </c>
@@ -1369,39 +1178,48 @@
       <c r="E6" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="4" t="n">
         <v>40</v>
       </c>
       <c r="G6" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H6" xr:uid="{00000000-0009-0000-0000-000009000000}"/>
+  <autoFilter ref="A1:H6"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="48.42578125" customWidth="1"/>
-    <col min="5" max="5" width="50.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="50.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1427,7 +1245,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1443,12 +1261,12 @@
       <c r="E2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="4" t="n">
         <v>10</v>
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1464,12 +1282,12 @@
       <c r="E3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="4" t="n">
         <v>8</v>
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1485,12 +1303,12 @@
       <c r="E4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="4" t="n">
         <v>6</v>
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1506,12 +1324,12 @@
       <c r="E5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="4" t="n">
         <v>12</v>
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1527,12 +1345,12 @@
       <c r="E6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="4" t="n">
         <v>10</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1548,12 +1366,12 @@
       <c r="E7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="4" t="n">
         <v>8</v>
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1569,12 +1387,12 @@
       <c r="E8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="4" t="n">
         <v>12</v>
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1590,12 +1408,12 @@
       <c r="E9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="4" t="n">
         <v>10</v>
       </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1611,38 +1429,47 @@
       <c r="E10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="4" t="n">
         <v>8</v>
       </c>
       <c r="G10" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H10" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:H10"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="55.42578125" customWidth="1"/>
-    <col min="5" max="5" width="58.28515625" customWidth="1"/>
-    <col min="6" max="7" width="12.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1668,7 +1495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1684,12 +1511,12 @@
       <c r="E2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="5" t="n">
         <v>8</v>
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1705,12 +1532,12 @@
       <c r="E3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="5" t="n">
         <v>10</v>
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1726,12 +1553,12 @@
       <c r="E4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="5" t="n">
         <v>12</v>
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1747,12 +1574,12 @@
       <c r="E5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="5" t="n">
         <v>8</v>
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1768,12 +1595,12 @@
       <c r="E6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="5" t="n">
         <v>12</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1789,12 +1616,12 @@
       <c r="E7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="5" t="n">
         <v>10</v>
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1810,12 +1637,12 @@
       <c r="E8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="5" t="n">
         <v>14</v>
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1831,12 +1658,12 @@
       <c r="E9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="5" t="n">
         <v>16</v>
       </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1852,12 +1679,12 @@
       <c r="E10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="5" t="n">
         <v>10</v>
       </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1873,12 +1700,12 @@
       <c r="E11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1894,37 +1721,46 @@
       <c r="E12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="5" t="n">
         <v>12</v>
       </c>
       <c r="G12" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H12" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:H12"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" customWidth="1"/>
-    <col min="5" max="5" width="43.5703125" customWidth="1"/>
-    <col min="6" max="8" width="18" style="1" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1950,7 +1786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>49</v>
       </c>
@@ -1966,13 +1802,13 @@
       <c r="E2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>54</v>
       </c>
@@ -1988,13 +1824,13 @@
       <c r="E3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>54</v>
       </c>
@@ -2010,13 +1846,13 @@
       <c r="E4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -2032,13 +1868,13 @@
       <c r="E5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>49</v>
       </c>
@@ -2054,13 +1890,13 @@
       <c r="E6" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>54</v>
       </c>
@@ -2076,13 +1912,13 @@
       <c r="E7" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -2098,13 +1934,13 @@
       <c r="E8" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
@@ -2120,13 +1956,13 @@
       <c r="E9" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>54</v>
       </c>
@@ -2142,13 +1978,13 @@
       <c r="E10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>54</v>
       </c>
@@ -2164,13 +2000,13 @@
       <c r="E11" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -2186,13 +2022,13 @@
       <c r="E12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>49</v>
       </c>
@@ -2208,13 +2044,13 @@
       <c r="E13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>54</v>
       </c>
@@ -2230,13 +2066,13 @@
       <c r="E14" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -2252,39 +2088,48 @@
       <c r="E15" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H15" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A1:H15"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="true">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" customWidth="1"/>
-    <col min="6" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2310,7 +2155,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
@@ -2326,12 +2171,14 @@
       <c r="E2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="5">
-        <v>8</v>
-      </c>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="F2" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -2347,12 +2194,12 @@
       <c r="E3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>54</v>
       </c>
@@ -2368,12 +2215,14 @@
       <c r="E4" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="5">
-        <v>4</v>
-      </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="F4" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -2389,12 +2238,12 @@
       <c r="E5" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
@@ -2410,12 +2259,14 @@
       <c r="E6" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="G6" s="5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -2431,12 +2282,12 @@
       <c r="E7" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>54</v>
       </c>
@@ -2452,12 +2303,14 @@
       <c r="E8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F8" s="5">
-        <v>4</v>
-      </c>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="F8" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -2473,12 +2326,12 @@
       <c r="E9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>54</v>
       </c>
@@ -2494,12 +2347,14 @@
       <c r="E10" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="G10" s="5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -2515,12 +2370,12 @@
       <c r="E11" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>54</v>
       </c>
@@ -2536,12 +2391,14 @@
       <c r="E12" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="5">
-        <v>8</v>
-      </c>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="F12" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
@@ -2557,12 +2414,12 @@
       <c r="E13" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>54</v>
       </c>
@@ -2578,12 +2435,14 @@
       <c r="E14" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="G14" s="5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -2599,12 +2458,12 @@
       <c r="E15" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>54</v>
       </c>
@@ -2620,12 +2479,14 @@
       <c r="E16" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="G16" s="5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
@@ -2641,12 +2502,12 @@
       <c r="E17" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>54</v>
       </c>
@@ -2662,12 +2523,14 @@
       <c r="E18" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="G18" s="5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>8</v>
       </c>
@@ -2683,12 +2546,12 @@
       <c r="E19" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>54</v>
       </c>
@@ -2704,12 +2567,14 @@
       <c r="E20" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F20" s="5">
-        <v>4</v>
-      </c>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="F20" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G20" s="5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
@@ -2725,41 +2590,55 @@
       <c r="E21" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G21" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H21" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A1:H21">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Backend Developer"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="true">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="42" customWidth="1"/>
-    <col min="6" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.85"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2785,7 +2664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1">
+    <row r="2" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>49</v>
       </c>
@@ -2801,12 +2680,12 @@
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="5" t="n">
         <v>8</v>
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>54</v>
       </c>
@@ -2822,12 +2701,12 @@
       <c r="E3" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="5" t="n">
         <v>10</v>
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -2843,12 +2722,12 @@
       <c r="E4" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>107</v>
       </c>
@@ -2864,14 +2743,14 @@
       <c r="E5" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="5">
-        <v>4</v>
-      </c>
-      <c r="G5" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" hidden="1">
+      <c r="F5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>49</v>
       </c>
@@ -2887,12 +2766,12 @@
       <c r="E6" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>54</v>
       </c>
@@ -2908,12 +2787,12 @@
       <c r="E7" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -2929,12 +2808,12 @@
       <c r="E8" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>107</v>
       </c>
@@ -2950,14 +2829,14 @@
       <c r="E9" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F9" s="5">
-        <v>4</v>
-      </c>
-      <c r="G9" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" hidden="1">
+      <c r="F9" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>54</v>
       </c>
@@ -2973,12 +2852,12 @@
       <c r="E10" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:8" hidden="1">
+    <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>54</v>
       </c>
@@ -2994,12 +2873,12 @@
       <c r="E11" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:8" hidden="1">
+    <row r="12" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -3015,12 +2894,12 @@
       <c r="E12" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>107</v>
       </c>
@@ -3036,14 +2915,14 @@
       <c r="E13" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="5" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>49</v>
       </c>
@@ -3059,12 +2938,12 @@
       <c r="E14" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>54</v>
       </c>
@@ -3080,12 +2959,12 @@
       <c r="E15" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -3101,12 +2980,12 @@
       <c r="E16" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>107</v>
       </c>
@@ -3122,14 +3001,14 @@
       <c r="E17" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="5" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
+    <row r="18" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>49</v>
       </c>
@@ -3145,12 +3024,12 @@
       <c r="E18" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" hidden="1">
+    <row r="19" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>54</v>
       </c>
@@ -3166,12 +3045,12 @@
       <c r="E19" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" hidden="1">
+    <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
@@ -3187,12 +3066,12 @@
       <c r="E20" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" hidden="1">
+    <row r="21" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>49</v>
       </c>
@@ -3208,12 +3087,12 @@
       <c r="E21" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" hidden="1">
+    <row r="22" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>54</v>
       </c>
@@ -3229,12 +3108,12 @@
       <c r="E22" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" hidden="1">
+    <row r="23" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
         <v>8</v>
       </c>
@@ -3250,12 +3129,12 @@
       <c r="E23" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" hidden="1">
+    <row r="24" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>49</v>
       </c>
@@ -3271,12 +3150,12 @@
       <c r="E24" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" hidden="1">
+    <row r="25" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
         <v>54</v>
       </c>
@@ -3292,12 +3171,12 @@
       <c r="E25" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" hidden="1">
+    <row r="26" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
         <v>8</v>
       </c>
@@ -3313,45 +3192,53 @@
       <c r="E26" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G26" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H26" xr:uid="{00000000-0009-0000-0000-000005000000}">
+  <autoFilter ref="A1:H26">
     <filterColumn colId="0">
       <filters>
         <filter val="Project Manager"/>
       </filters>
     </filterColumn>
   </autoFilter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="true">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" customWidth="1"/>
-    <col min="6" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3377,7 +3264,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1">
+    <row r="2" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>49</v>
       </c>
@@ -3393,12 +3280,12 @@
       <c r="E2" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="7" t="n">
         <v>6</v>
       </c>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>49</v>
       </c>
@@ -3414,12 +3301,12 @@
       <c r="E3" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="7" t="n">
         <v>12</v>
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>54</v>
       </c>
@@ -3435,12 +3322,12 @@
       <c r="E4" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="7" t="n">
         <v>8</v>
       </c>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:8" hidden="1">
+    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
         <v>54</v>
       </c>
@@ -3456,12 +3343,12 @@
       <c r="E5" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="7" t="n">
         <v>6</v>
       </c>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
         <v>49</v>
       </c>
@@ -3477,12 +3364,12 @@
       <c r="E6" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="7" t="n">
         <v>10</v>
       </c>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>49</v>
       </c>
@@ -3498,12 +3385,12 @@
       <c r="E7" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="7" t="n">
         <v>12</v>
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>49</v>
       </c>
@@ -3519,12 +3406,12 @@
       <c r="E8" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="7" t="n">
         <v>8</v>
       </c>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
         <v>54</v>
       </c>
@@ -3540,12 +3427,12 @@
       <c r="E9" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="7" t="n">
         <v>8</v>
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>49</v>
       </c>
@@ -3561,12 +3448,12 @@
       <c r="E10" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="7" t="n">
         <v>8</v>
       </c>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:8" hidden="1">
+    <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>54</v>
       </c>
@@ -3582,12 +3469,12 @@
       <c r="E11" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="7" t="n">
         <v>10</v>
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:8" hidden="1">
+    <row r="12" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>49</v>
       </c>
@@ -3603,12 +3490,12 @@
       <c r="E12" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="7" t="n">
         <v>8</v>
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>54</v>
       </c>
@@ -3624,12 +3511,12 @@
       <c r="E13" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="7" t="n">
         <v>10</v>
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
         <v>49</v>
       </c>
@@ -3645,12 +3532,12 @@
       <c r="E14" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="7" t="n">
         <v>8</v>
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
         <v>54</v>
       </c>
@@ -3666,12 +3553,12 @@
       <c r="E15" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="7" t="n">
         <v>8</v>
       </c>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
         <v>49</v>
       </c>
@@ -3687,12 +3574,12 @@
       <c r="E16" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="7" t="n">
         <v>8</v>
       </c>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" hidden="1">
+    <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
         <v>54</v>
       </c>
@@ -3708,12 +3595,12 @@
       <c r="E17" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="7" t="n">
         <v>8</v>
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" hidden="1">
+    <row r="18" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
         <v>49</v>
       </c>
@@ -3729,12 +3616,12 @@
       <c r="E18" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="7" t="n">
         <v>8</v>
       </c>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" hidden="1">
+    <row r="19" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
         <v>54</v>
       </c>
@@ -3750,12 +3637,12 @@
       <c r="E19" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="7" t="n">
         <v>8</v>
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
         <v>107</v>
       </c>
@@ -3771,46 +3658,55 @@
       <c r="E20" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="7" t="n">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H20" xr:uid="{00000000-0009-0000-0000-000006000000}">
+  <autoFilter ref="A1:H20">
     <filterColumn colId="0">
       <filters>
         <filter val="Project Manager"/>
       </filters>
     </filterColumn>
   </autoFilter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="4" width="34.85546875" customWidth="1"/>
-    <col min="5" max="5" width="53.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="34.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="53.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.85"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3836,7 +3732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>107</v>
       </c>
@@ -3852,14 +3748,14 @@
       <c r="E2" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="5" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>107</v>
       </c>
@@ -3875,14 +3771,14 @@
       <c r="E3" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="5" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>107</v>
       </c>
@@ -3898,14 +3794,14 @@
       <c r="E4" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="5" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>107</v>
       </c>
@@ -3921,39 +3817,48 @@
       <c r="E5" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="5" t="n">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H5" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
+  <autoFilter ref="A1:H5"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="53.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="53.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3979,7 +3884,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>107</v>
       </c>
@@ -3995,14 +3900,14 @@
       <c r="E2" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="5" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>107</v>
       </c>
@@ -4018,14 +3923,14 @@
       <c r="E3" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="5" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>107</v>
       </c>
@@ -4041,17 +3946,23 @@
       <c r="E4" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="5" t="n">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H4" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
+  <autoFilter ref="A1:H4"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>